<commit_message>
building the json wrapper
</commit_message>
<xml_diff>
--- a/JSON/data/reports.xlsx
+++ b/JSON/data/reports.xlsx
@@ -5,25 +5,102 @@
     <workbookView tabRatio="600" windowHeight="14980" windowWidth="25600" xWindow="0" yWindow="1080"/>
   </bookViews>
   <sheets>
-    <sheet name="FirstReport" sheetId="1" r:id="RsBMXRmxQWVcmIsLn"/>
-    <sheet name="SecondReport" sheetId="2" r:id="RE3HjNftyvS2CYBXQ"/>
+    <sheet name="monthlySummary" sheetId="1" r:id="R2GwSDhmuFH9CEcLh"/>
+    <sheet name="monthlyTop20Detail" sheetId="2" r:id="RhDvj1Rs7aJmLMlrU"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+  <si>
+    <t>Employee Number</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Total Achievements</t>
+  </si>
+  <si>
+    <t>Total Kudos</t>
+  </si>
+  <si>
+    <t>x1y2</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2014-11-20T06:59:26.403Z</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>20141119, RMB Demo1, for having a Microsoft meltdown.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="26"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -47,8 +124,20 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf applyNumberFormat="0" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0"/>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf applyNumberFormat="0" applyFill="0" applyFont="1" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -66,7 +155,42 @@
     <col customWidth="1" max="1" min="1" width="20"/>
   </cols>
   <sheetData>
-    <row r="1"/>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
@@ -85,6 +209,30 @@
   </cols>
   <sheetData>
     <row r="1"/>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>